<commit_message>
Add calculation of current dates for the example file example_ubw_report
</commit_message>
<xml_diff>
--- a/budgeteer-ubw-importer/src/main/resources/example_ubw_report.xlsx
+++ b/budgeteer-ubw-importer/src/main/resources/example_ubw_report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trzpiot\Documents\Workspace\Examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trzpiot\Documents\Workspace\budgeteer\budgeteer-ubw-importer\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -3183,7 +3183,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3291,10 +3291,7 @@
       <c r="C4" s="113" t="s">
         <v>106</v>
       </c>
-      <c r="D4" s="114">
-        <f ca="1">TODAY()-39</f>
-        <v>43283</v>
-      </c>
+      <c r="D4" s="114"/>
       <c r="E4" s="113"/>
       <c r="F4" s="113"/>
       <c r="G4" s="113">
@@ -3330,10 +3327,7 @@
       <c r="C5" s="113" t="s">
         <v>106</v>
       </c>
-      <c r="D5" s="114">
-        <f ca="1">TODAY()-38</f>
-        <v>43284</v>
-      </c>
+      <c r="D5" s="114"/>
       <c r="E5" s="113"/>
       <c r="F5" s="113"/>
       <c r="G5" s="113">
@@ -3369,10 +3363,7 @@
       <c r="C6" s="113" t="s">
         <v>106</v>
       </c>
-      <c r="D6" s="114">
-        <f ca="1">TODAY()-37</f>
-        <v>43285</v>
-      </c>
+      <c r="D6" s="114"/>
       <c r="E6" s="113"/>
       <c r="F6" s="113"/>
       <c r="G6" s="113">
@@ -3408,10 +3399,7 @@
       <c r="C7" s="113" t="s">
         <v>106</v>
       </c>
-      <c r="D7" s="114">
-        <f t="shared" ref="D7:D31" ca="1" si="0">D8-IF(WEEKDAY(D8,2)=1,3,1)</f>
-        <v>43286</v>
-      </c>
+      <c r="D7" s="114"/>
       <c r="E7" s="113"/>
       <c r="F7" s="113"/>
       <c r="G7" s="113">
@@ -3447,10 +3435,7 @@
       <c r="C8" s="113" t="s">
         <v>106</v>
       </c>
-      <c r="D8" s="114">
-        <f t="shared" ca="1" si="0"/>
-        <v>43287</v>
-      </c>
+      <c r="D8" s="114"/>
       <c r="E8" s="113"/>
       <c r="F8" s="113"/>
       <c r="G8" s="113">
@@ -3486,10 +3471,7 @@
       <c r="C9" s="113" t="s">
         <v>106</v>
       </c>
-      <c r="D9" s="114">
-        <f t="shared" ca="1" si="0"/>
-        <v>43290</v>
-      </c>
+      <c r="D9" s="114"/>
       <c r="E9" s="113"/>
       <c r="F9" s="113"/>
       <c r="G9" s="113">
@@ -3525,10 +3507,7 @@
       <c r="C10" s="113" t="s">
         <v>106</v>
       </c>
-      <c r="D10" s="114">
-        <f t="shared" ca="1" si="0"/>
-        <v>43291</v>
-      </c>
+      <c r="D10" s="114"/>
       <c r="E10" s="113"/>
       <c r="F10" s="113"/>
       <c r="G10" s="113">
@@ -3564,10 +3543,7 @@
       <c r="C11" s="113" t="s">
         <v>106</v>
       </c>
-      <c r="D11" s="114">
-        <f t="shared" ca="1" si="0"/>
-        <v>43292</v>
-      </c>
+      <c r="D11" s="114"/>
       <c r="E11" s="113"/>
       <c r="F11" s="113"/>
       <c r="G11" s="113">
@@ -3603,10 +3579,7 @@
       <c r="C12" s="113" t="s">
         <v>106</v>
       </c>
-      <c r="D12" s="114">
-        <f t="shared" ca="1" si="0"/>
-        <v>43293</v>
-      </c>
+      <c r="D12" s="114"/>
       <c r="E12" s="113"/>
       <c r="F12" s="113"/>
       <c r="G12" s="113">
@@ -3642,10 +3615,7 @@
       <c r="C13" s="113" t="s">
         <v>106</v>
       </c>
-      <c r="D13" s="114">
-        <f t="shared" ca="1" si="0"/>
-        <v>43294</v>
-      </c>
+      <c r="D13" s="114"/>
       <c r="E13" s="113"/>
       <c r="F13" s="113"/>
       <c r="G13" s="113">
@@ -3681,10 +3651,7 @@
       <c r="C14" s="113" t="s">
         <v>106</v>
       </c>
-      <c r="D14" s="114">
-        <f t="shared" ca="1" si="0"/>
-        <v>43297</v>
-      </c>
+      <c r="D14" s="114"/>
       <c r="E14" s="113"/>
       <c r="F14" s="113"/>
       <c r="G14" s="113">
@@ -3720,10 +3687,7 @@
       <c r="C15" s="113" t="s">
         <v>106</v>
       </c>
-      <c r="D15" s="114">
-        <f t="shared" ca="1" si="0"/>
-        <v>43298</v>
-      </c>
+      <c r="D15" s="114"/>
       <c r="E15" s="113"/>
       <c r="F15" s="113"/>
       <c r="G15" s="113">
@@ -3759,10 +3723,7 @@
       <c r="C16" s="113" t="s">
         <v>106</v>
       </c>
-      <c r="D16" s="114">
-        <f t="shared" ca="1" si="0"/>
-        <v>43299</v>
-      </c>
+      <c r="D16" s="114"/>
       <c r="E16" s="113"/>
       <c r="F16" s="113"/>
       <c r="G16" s="113">
@@ -3796,10 +3757,7 @@
       <c r="C17" s="113" t="s">
         <v>106</v>
       </c>
-      <c r="D17" s="114">
-        <f t="shared" ca="1" si="0"/>
-        <v>43300</v>
-      </c>
+      <c r="D17" s="114"/>
       <c r="E17" s="113"/>
       <c r="F17" s="113"/>
       <c r="G17" s="113">
@@ -3833,10 +3791,7 @@
       <c r="C18" s="113" t="s">
         <v>106</v>
       </c>
-      <c r="D18" s="114">
-        <f t="shared" ca="1" si="0"/>
-        <v>43301</v>
-      </c>
+      <c r="D18" s="114"/>
       <c r="E18" s="113"/>
       <c r="F18" s="113"/>
       <c r="G18" s="113">
@@ -3870,10 +3825,7 @@
       <c r="C19" s="113" t="s">
         <v>106</v>
       </c>
-      <c r="D19" s="114">
-        <f t="shared" ca="1" si="0"/>
-        <v>43304</v>
-      </c>
+      <c r="D19" s="114"/>
       <c r="E19" s="113"/>
       <c r="F19" s="113"/>
       <c r="G19" s="113">
@@ -3909,10 +3861,7 @@
       <c r="C20" s="113" t="s">
         <v>106</v>
       </c>
-      <c r="D20" s="114">
-        <f t="shared" ca="1" si="0"/>
-        <v>43305</v>
-      </c>
+      <c r="D20" s="114"/>
       <c r="E20" s="113"/>
       <c r="F20" s="113"/>
       <c r="G20" s="113">
@@ -3948,10 +3897,7 @@
       <c r="C21" s="113" t="s">
         <v>106</v>
       </c>
-      <c r="D21" s="114">
-        <f t="shared" ca="1" si="0"/>
-        <v>43306</v>
-      </c>
+      <c r="D21" s="114"/>
       <c r="E21" s="113"/>
       <c r="F21" s="113"/>
       <c r="G21" s="113">
@@ -3987,10 +3933,7 @@
       <c r="C22" s="113" t="s">
         <v>106</v>
       </c>
-      <c r="D22" s="114">
-        <f t="shared" ca="1" si="0"/>
-        <v>43307</v>
-      </c>
+      <c r="D22" s="114"/>
       <c r="E22" s="113"/>
       <c r="F22" s="113"/>
       <c r="G22" s="113">
@@ -4026,10 +3969,7 @@
       <c r="C23" s="113" t="s">
         <v>106</v>
       </c>
-      <c r="D23" s="114">
-        <f t="shared" ca="1" si="0"/>
-        <v>43308</v>
-      </c>
+      <c r="D23" s="114"/>
       <c r="E23" s="113"/>
       <c r="F23" s="113"/>
       <c r="G23" s="113">
@@ -4065,10 +4005,7 @@
       <c r="C24" s="113" t="s">
         <v>106</v>
       </c>
-      <c r="D24" s="114">
-        <f t="shared" ca="1" si="0"/>
-        <v>43311</v>
-      </c>
+      <c r="D24" s="114"/>
       <c r="E24" s="113"/>
       <c r="F24" s="113"/>
       <c r="G24" s="113">
@@ -4102,10 +4039,7 @@
       <c r="C25" s="113" t="s">
         <v>106</v>
       </c>
-      <c r="D25" s="114">
-        <f t="shared" ca="1" si="0"/>
-        <v>43312</v>
-      </c>
+      <c r="D25" s="114"/>
       <c r="E25" s="113"/>
       <c r="F25" s="113"/>
       <c r="G25" s="113">
@@ -4141,10 +4075,7 @@
       <c r="C26" s="113" t="s">
         <v>106</v>
       </c>
-      <c r="D26" s="114">
-        <f t="shared" ca="1" si="0"/>
-        <v>43313</v>
-      </c>
+      <c r="D26" s="114"/>
       <c r="E26" s="113"/>
       <c r="F26" s="113"/>
       <c r="G26" s="113">
@@ -4180,10 +4111,7 @@
       <c r="C27" s="113" t="s">
         <v>106</v>
       </c>
-      <c r="D27" s="114">
-        <f t="shared" ca="1" si="0"/>
-        <v>43314</v>
-      </c>
+      <c r="D27" s="114"/>
       <c r="E27" s="113"/>
       <c r="F27" s="113"/>
       <c r="G27" s="113">
@@ -4217,10 +4145,7 @@
       <c r="C28" s="113" t="s">
         <v>106</v>
       </c>
-      <c r="D28" s="114">
-        <f t="shared" ca="1" si="0"/>
-        <v>43315</v>
-      </c>
+      <c r="D28" s="114"/>
       <c r="E28" s="113"/>
       <c r="F28" s="113"/>
       <c r="G28" s="113">
@@ -4256,10 +4181,7 @@
       <c r="C29" s="113" t="s">
         <v>106</v>
       </c>
-      <c r="D29" s="114">
-        <f t="shared" ca="1" si="0"/>
-        <v>43318</v>
-      </c>
+      <c r="D29" s="114"/>
       <c r="E29" s="113"/>
       <c r="F29" s="113"/>
       <c r="G29" s="113">
@@ -4295,10 +4217,7 @@
       <c r="C30" s="113" t="s">
         <v>106</v>
       </c>
-      <c r="D30" s="114">
-        <f t="shared" ca="1" si="0"/>
-        <v>43319</v>
-      </c>
+      <c r="D30" s="114"/>
       <c r="E30" s="113"/>
       <c r="F30" s="113"/>
       <c r="G30" s="113">
@@ -4334,10 +4253,7 @@
       <c r="C31" s="113" t="s">
         <v>106</v>
       </c>
-      <c r="D31" s="114">
-        <f t="shared" ca="1" si="0"/>
-        <v>43320</v>
-      </c>
+      <c r="D31" s="114"/>
       <c r="E31" s="113"/>
       <c r="F31" s="113"/>
       <c r="G31" s="113">
@@ -4373,10 +4289,7 @@
       <c r="C32" s="113" t="s">
         <v>106</v>
       </c>
-      <c r="D32" s="114">
-        <f ca="1">D33-IF(WEEKDAY(D33,2)=1,3,1)</f>
-        <v>43321</v>
-      </c>
+      <c r="D32" s="114"/>
       <c r="E32" s="113"/>
       <c r="F32" s="113"/>
       <c r="G32" s="113">
@@ -4410,10 +4323,7 @@
       <c r="C33" s="113" t="s">
         <v>106</v>
       </c>
-      <c r="D33" s="114">
-        <f ca="1">TODAY()</f>
-        <v>43322</v>
-      </c>
+      <c r="D33" s="114"/>
       <c r="E33" s="113"/>
       <c r="F33" s="113"/>
       <c r="G33" s="113">
@@ -4449,10 +4359,7 @@
       <c r="C34" s="113" t="s">
         <v>108</v>
       </c>
-      <c r="D34" s="114">
-        <f t="shared" ref="D34:D38" ca="1" si="1">D35-IF(WEEKDAY(D35,2)=1,3,1)</f>
-        <v>43283</v>
-      </c>
+      <c r="D34" s="114"/>
       <c r="E34" s="113"/>
       <c r="F34" s="113"/>
       <c r="G34" s="113">
@@ -4488,10 +4395,7 @@
       <c r="C35" s="113" t="s">
         <v>108</v>
       </c>
-      <c r="D35" s="114">
-        <f t="shared" ca="1" si="1"/>
-        <v>43284</v>
-      </c>
+      <c r="D35" s="114"/>
       <c r="E35" s="113"/>
       <c r="F35" s="113"/>
       <c r="G35" s="113">
@@ -4527,10 +4431,7 @@
       <c r="C36" s="113" t="s">
         <v>108</v>
       </c>
-      <c r="D36" s="114">
-        <f t="shared" ca="1" si="1"/>
-        <v>43285</v>
-      </c>
+      <c r="D36" s="114"/>
       <c r="E36" s="113"/>
       <c r="F36" s="113"/>
       <c r="G36" s="113">
@@ -4566,10 +4467,7 @@
       <c r="C37" s="113" t="s">
         <v>108</v>
       </c>
-      <c r="D37" s="114">
-        <f t="shared" ca="1" si="1"/>
-        <v>43286</v>
-      </c>
+      <c r="D37" s="114"/>
       <c r="E37" s="113"/>
       <c r="F37" s="113"/>
       <c r="G37" s="113">
@@ -4605,10 +4503,7 @@
       <c r="C38" s="113" t="s">
         <v>108</v>
       </c>
-      <c r="D38" s="114">
-        <f t="shared" ca="1" si="1"/>
-        <v>43287</v>
-      </c>
+      <c r="D38" s="114"/>
       <c r="E38" s="113"/>
       <c r="F38" s="113"/>
       <c r="G38" s="113">
@@ -4644,10 +4539,7 @@
       <c r="C39" s="113" t="s">
         <v>108</v>
       </c>
-      <c r="D39" s="114">
-        <f t="shared" ref="D39:D48" ca="1" si="2">D40-IF(WEEKDAY(D40,2)=1,3,1)</f>
-        <v>43290</v>
-      </c>
+      <c r="D39" s="114"/>
       <c r="E39" s="113"/>
       <c r="F39" s="113"/>
       <c r="G39" s="113">
@@ -4683,10 +4575,7 @@
       <c r="C40" s="113" t="s">
         <v>108</v>
       </c>
-      <c r="D40" s="114">
-        <f t="shared" ca="1" si="2"/>
-        <v>43291</v>
-      </c>
+      <c r="D40" s="114"/>
       <c r="E40" s="113"/>
       <c r="F40" s="113"/>
       <c r="G40" s="113">
@@ -4722,10 +4611,7 @@
       <c r="C41" s="113" t="s">
         <v>108</v>
       </c>
-      <c r="D41" s="114">
-        <f t="shared" ca="1" si="2"/>
-        <v>43292</v>
-      </c>
+      <c r="D41" s="114"/>
       <c r="E41" s="113"/>
       <c r="F41" s="113"/>
       <c r="G41" s="113">
@@ -4761,10 +4647,7 @@
       <c r="C42" s="113" t="s">
         <v>108</v>
       </c>
-      <c r="D42" s="114">
-        <f t="shared" ca="1" si="2"/>
-        <v>43293</v>
-      </c>
+      <c r="D42" s="114"/>
       <c r="E42" s="113"/>
       <c r="F42" s="113"/>
       <c r="G42" s="113">
@@ -4800,10 +4683,7 @@
       <c r="C43" s="113" t="s">
         <v>108</v>
       </c>
-      <c r="D43" s="114">
-        <f t="shared" ca="1" si="2"/>
-        <v>43294</v>
-      </c>
+      <c r="D43" s="114"/>
       <c r="E43" s="113"/>
       <c r="F43" s="113"/>
       <c r="G43" s="113">
@@ -4839,10 +4719,7 @@
       <c r="C44" s="113" t="s">
         <v>108</v>
       </c>
-      <c r="D44" s="114">
-        <f t="shared" ca="1" si="2"/>
-        <v>43297</v>
-      </c>
+      <c r="D44" s="114"/>
       <c r="E44" s="113"/>
       <c r="F44" s="113"/>
       <c r="G44" s="113">
@@ -4878,10 +4755,7 @@
       <c r="C45" s="113" t="s">
         <v>108</v>
       </c>
-      <c r="D45" s="114">
-        <f t="shared" ca="1" si="2"/>
-        <v>43298</v>
-      </c>
+      <c r="D45" s="114"/>
       <c r="E45" s="113"/>
       <c r="F45" s="113"/>
       <c r="G45" s="113">
@@ -4917,10 +4791,7 @@
       <c r="C46" s="113" t="s">
         <v>108</v>
       </c>
-      <c r="D46" s="114">
-        <f t="shared" ca="1" si="2"/>
-        <v>43299</v>
-      </c>
+      <c r="D46" s="114"/>
       <c r="E46" s="113"/>
       <c r="F46" s="113"/>
       <c r="G46" s="113">
@@ -4956,10 +4827,7 @@
       <c r="C47" s="113" t="s">
         <v>108</v>
       </c>
-      <c r="D47" s="114">
-        <f t="shared" ca="1" si="2"/>
-        <v>43300</v>
-      </c>
+      <c r="D47" s="114"/>
       <c r="E47" s="113"/>
       <c r="F47" s="113"/>
       <c r="G47" s="113">
@@ -4995,10 +4863,7 @@
       <c r="C48" s="113" t="s">
         <v>108</v>
       </c>
-      <c r="D48" s="114">
-        <f t="shared" ca="1" si="2"/>
-        <v>43301</v>
-      </c>
+      <c r="D48" s="114"/>
       <c r="E48" s="113"/>
       <c r="F48" s="113"/>
       <c r="G48" s="113">
@@ -5034,10 +4899,7 @@
       <c r="C49" s="113" t="s">
         <v>108</v>
       </c>
-      <c r="D49" s="114">
-        <f t="shared" ref="D49:D60" ca="1" si="3">D50-IF(WEEKDAY(D50,2)=1,3,1)</f>
-        <v>43304</v>
-      </c>
+      <c r="D49" s="114"/>
       <c r="E49" s="113"/>
       <c r="F49" s="113"/>
       <c r="G49" s="113">
@@ -5073,10 +4935,7 @@
       <c r="C50" s="113" t="s">
         <v>108</v>
       </c>
-      <c r="D50" s="114">
-        <f t="shared" ca="1" si="3"/>
-        <v>43305</v>
-      </c>
+      <c r="D50" s="114"/>
       <c r="E50" s="113"/>
       <c r="F50" s="113"/>
       <c r="G50" s="113">
@@ -5112,10 +4971,7 @@
       <c r="C51" s="113" t="s">
         <v>108</v>
       </c>
-      <c r="D51" s="114">
-        <f t="shared" ca="1" si="3"/>
-        <v>43306</v>
-      </c>
+      <c r="D51" s="114"/>
       <c r="E51" s="113"/>
       <c r="F51" s="113"/>
       <c r="G51" s="113">
@@ -5151,10 +5007,7 @@
       <c r="C52" s="113" t="s">
         <v>108</v>
       </c>
-      <c r="D52" s="114">
-        <f t="shared" ca="1" si="3"/>
-        <v>43307</v>
-      </c>
+      <c r="D52" s="114"/>
       <c r="E52" s="113"/>
       <c r="F52" s="113"/>
       <c r="G52" s="113">
@@ -5190,10 +5043,7 @@
       <c r="C53" s="113" t="s">
         <v>108</v>
       </c>
-      <c r="D53" s="114">
-        <f t="shared" ca="1" si="3"/>
-        <v>43308</v>
-      </c>
+      <c r="D53" s="114"/>
       <c r="E53" s="113"/>
       <c r="F53" s="113"/>
       <c r="G53" s="113">
@@ -5229,10 +5079,7 @@
       <c r="C54" s="113" t="s">
         <v>108</v>
       </c>
-      <c r="D54" s="114">
-        <f t="shared" ca="1" si="3"/>
-        <v>43311</v>
-      </c>
+      <c r="D54" s="114"/>
       <c r="E54" s="113"/>
       <c r="F54" s="113"/>
       <c r="G54" s="113">
@@ -5268,10 +5115,7 @@
       <c r="C55" s="113" t="s">
         <v>108</v>
       </c>
-      <c r="D55" s="114">
-        <f t="shared" ca="1" si="3"/>
-        <v>43312</v>
-      </c>
+      <c r="D55" s="114"/>
       <c r="E55" s="113"/>
       <c r="F55" s="113"/>
       <c r="G55" s="113">
@@ -5307,10 +5151,7 @@
       <c r="C56" s="113" t="s">
         <v>108</v>
       </c>
-      <c r="D56" s="114">
-        <f t="shared" ca="1" si="3"/>
-        <v>43313</v>
-      </c>
+      <c r="D56" s="114"/>
       <c r="E56" s="113"/>
       <c r="F56" s="113"/>
       <c r="G56" s="113">
@@ -5346,10 +5187,7 @@
       <c r="C57" s="113" t="s">
         <v>108</v>
       </c>
-      <c r="D57" s="114">
-        <f t="shared" ca="1" si="3"/>
-        <v>43314</v>
-      </c>
+      <c r="D57" s="114"/>
       <c r="E57" s="113"/>
       <c r="F57" s="113"/>
       <c r="G57" s="113">
@@ -5385,10 +5223,7 @@
       <c r="C58" s="113" t="s">
         <v>108</v>
       </c>
-      <c r="D58" s="114">
-        <f t="shared" ca="1" si="3"/>
-        <v>43315</v>
-      </c>
+      <c r="D58" s="114"/>
       <c r="E58" s="113"/>
       <c r="F58" s="113"/>
       <c r="G58" s="113">
@@ -5422,10 +5257,7 @@
       <c r="C59" s="113" t="s">
         <v>108</v>
       </c>
-      <c r="D59" s="114">
-        <f t="shared" ca="1" si="3"/>
-        <v>43318</v>
-      </c>
+      <c r="D59" s="114"/>
       <c r="E59" s="113"/>
       <c r="F59" s="113"/>
       <c r="G59" s="113">
@@ -5459,10 +5291,7 @@
       <c r="C60" s="113" t="s">
         <v>108</v>
       </c>
-      <c r="D60" s="114">
-        <f t="shared" ca="1" si="3"/>
-        <v>43319</v>
-      </c>
+      <c r="D60" s="114"/>
       <c r="E60" s="113"/>
       <c r="F60" s="113"/>
       <c r="G60" s="113">
@@ -5496,10 +5325,7 @@
       <c r="C61" s="113" t="s">
         <v>108</v>
       </c>
-      <c r="D61" s="114">
-        <f ca="1">D62-IF(WEEKDAY(D62,2)=1,3,1)</f>
-        <v>43320</v>
-      </c>
+      <c r="D61" s="114"/>
       <c r="E61" s="113"/>
       <c r="F61" s="113"/>
       <c r="G61" s="113">
@@ -5533,10 +5359,7 @@
       <c r="C62" s="113" t="s">
         <v>108</v>
       </c>
-      <c r="D62" s="114">
-        <f ca="1">TODAY()-1</f>
-        <v>43321</v>
-      </c>
+      <c r="D62" s="114"/>
       <c r="E62" s="113"/>
       <c r="F62" s="113"/>
       <c r="G62" s="113">
@@ -5570,10 +5393,7 @@
       <c r="C63" s="113" t="s">
         <v>108</v>
       </c>
-      <c r="D63" s="114">
-        <f ca="1">TODAY()</f>
-        <v>43322</v>
-      </c>
+      <c r="D63" s="114"/>
       <c r="E63" s="113"/>
       <c r="F63" s="113"/>
       <c r="G63" s="113">
@@ -11840,9 +11660,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11994,26 +11817,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A553A998-B02F-4A44-B634-4323F20DC2E4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2500D75-6B13-4050-B65D-E203B093A8B3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1373898a-3781-4d30-8397-9da1a4eac464"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -12037,9 +11849,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2500D75-6B13-4050-B65D-E203B093A8B3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A553A998-B02F-4A44-B634-4323F20DC2E4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1373898a-3781-4d30-8397-9da1a4eac464"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>